<commit_message>
Cleaning Code, removing unwanted comments
</commit_message>
<xml_diff>
--- a/Documentation/Risk Assessment To Do.xlsx
+++ b/Documentation/Risk Assessment To Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\ToDoListProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF05FD27-175F-4245-8A86-3B82BE508F55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC43CE6-B515-4DFC-B994-159600A96B21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{8CB24F64-C717-488D-A877-05C866C4B332}"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="26827" windowHeight="12337" xr2:uid="{8CB24F64-C717-488D-A877-05C866C4B332}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>Project Name:</t>
   </si>
@@ -168,10 +168,43 @@
     <t>Application not compiling</t>
   </si>
   <si>
-    <t>This would effect the project heavily as the porject MVP requires that this has to be done</t>
-  </si>
-  <si>
     <t>Continuously test the project to ensure it does not fail</t>
+  </si>
+  <si>
+    <t>At the end of the project, the jar file would need to compile.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This would cause applications to not function properly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A </t>
+  </si>
+  <si>
+    <t>Buying external hard-drives and ensuring that I delete everything that is not needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family Emergency </t>
+  </si>
+  <si>
+    <t>This is something that I won't be able to predict or account for.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This can cause me to take some leave to deal with the emergency </t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>This would effect the project heavily as the project MVP requires that this has to be done</t>
+  </si>
+  <si>
+    <t>Laptop Memory Issues</t>
+  </si>
+  <si>
+    <t>As I am required to download more software's to be able to create project the memory issues might occur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensuring that I keep up top do with course information  being put in a video format or text. </t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672790C0-2960-4938-80FA-B969A373BC5B}">
   <dimension ref="A1:AM21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1327,7 +1360,7 @@
       <c r="W6" s="40"/>
       <c r="X6" s="41"/>
     </row>
-    <row r="7" spans="1:24" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:24" ht="92.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1338,7 +1371,9 @@
       <c r="C7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="E7" s="21"/>
       <c r="F7" s="31" t="s">
         <v>22</v>
@@ -1350,32 +1385,48 @@
         <v>22</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="91.9" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
+      <c r="B8" s="10">
+        <v>44410</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="31"/>
       <c r="G8" s="23"/>
       <c r="H8" s="21"/>
       <c r="I8" s="24"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="7"/>
+      <c r="J8" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="O8" s="20" t="s">
         <v>5</v>
       </c>
@@ -1391,23 +1442,39 @@
       <c r="W8" s="43"/>
       <c r="X8" s="44"/>
     </row>
-    <row r="9" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="9" spans="1:24" ht="91.9" x14ac:dyDescent="0.9">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="21"/>
+      <c r="B9" s="10">
+        <v>44441</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
       <c r="H9" s="21"/>
       <c r="I9" s="24"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="7"/>
+      <c r="J9" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="O9" s="29" t="s">
         <v>23</v>
       </c>
@@ -1703,21 +1770,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CB0BA5692D439F4BB79CC4D90864FB65" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a0b4bc8ff41ed1b65ab69efcd88df2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a228e58f-08c5-4e30-81dc-fb2ae1d06aa5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cccaba783f5d612f80b59805e7d0b95e" ns2:_="">
     <xsd:import namespace="a228e58f-08c5-4e30-81dc-fb2ae1d06aa5"/>
@@ -1895,24 +1947,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8350BFB4-A9D9-4E31-80BD-0DE15D9680ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADDABAF6-F01C-4289-9695-2F24BCAFA78E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26513C23-1B03-419F-B40E-B40C48D3FC52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1928,4 +1978,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADDABAF6-F01C-4289-9695-2F24BCAFA78E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8350BFB4-A9D9-4E31-80BD-0DE15D9680ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>